<commit_message>
fb logo in footer and csv delete last row
</commit_message>
<xml_diff>
--- a/build/odpowiedzi-komitetow.xlsx
+++ b/build/odpowiedzi-komitetow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Documents\03_Informatyka\01.FRONT-END\latarnik-wyborczy\gdanski-latarnik-wyborczy\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDD034F6-12CE-4335-8AAC-DC64811306B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A2D01E-9AD0-4A6D-A404-D4DE31A8385D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
-  <si>
-    <t>PIS</t>
-  </si>
-  <si>
-    <t>KO</t>
-  </si>
-  <si>
-    <t>WGD2050</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Kocham Gdańsk</t>
   </si>
@@ -159,6 +150,18 @@
   </si>
   <si>
     <t>Wyjaśnienia</t>
+  </si>
+  <si>
+    <t>Konfederacja</t>
+  </si>
+  <si>
+    <t>Koalicja Obywatelska</t>
+  </si>
+  <si>
+    <t>Prawo i Sprawiedliwość</t>
+  </si>
+  <si>
+    <t>Wspólna Gdańska Droga 2050</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,27 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -442,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H984"/>
+  <dimension ref="A1:I984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -457,35 +480,38 @@
     <col min="8" max="18" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2">
@@ -506,10 +532,13 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3">
@@ -530,10 +559,13 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4">
@@ -554,10 +586,13 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5">
@@ -578,10 +613,13 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6">
@@ -602,10 +640,13 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7">
@@ -626,10 +667,13 @@
       <c r="H7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8">
@@ -650,10 +694,13 @@
       <c r="H8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9">
@@ -674,10 +721,13 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10">
@@ -698,10 +748,13 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11">
@@ -722,10 +775,13 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12">
@@ -746,10 +802,13 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13">
@@ -770,10 +829,13 @@
       <c r="H13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14">
@@ -794,10 +856,13 @@
       <c r="H14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15">
@@ -818,10 +883,13 @@
       <c r="H15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16">
@@ -842,10 +910,13 @@
       <c r="H16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17">
@@ -866,10 +937,13 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18">
@@ -890,10 +964,13 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19">
@@ -914,10 +991,13 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20">
@@ -938,10 +1018,13 @@
       <c r="H20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21">
@@ -962,10 +1045,13 @@
       <c r="H21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22">
@@ -986,10 +1072,13 @@
       <c r="H22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23">
@@ -1010,10 +1099,13 @@
       <c r="H23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24">
@@ -1034,10 +1126,13 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25">
@@ -1058,10 +1153,13 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26">
@@ -1082,10 +1180,13 @@
       <c r="H26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27">
@@ -1106,10 +1207,13 @@
       <c r="H27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28">
@@ -1130,10 +1234,13 @@
       <c r="H28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29">
@@ -1154,10 +1261,13 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30">
@@ -1178,10 +1288,13 @@
       <c r="H30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31">
@@ -1202,10 +1315,13 @@
       <c r="H31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32">
@@ -1226,10 +1342,13 @@
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33">
@@ -1250,10 +1369,13 @@
       <c r="H33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34">
@@ -1274,21 +1396,24 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="I34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2227,7 +2352,12 @@
     <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="E2:E33 C2:D34 F2:H34">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I34">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>